<commit_message>
Removed squeeze functionality and testing
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttami001/Documents/forked_tbrs_opensource/trbs/src/vlinder/data/beerwiser/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aweijden002\Documents\tRBS anne\Fork Ruen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D84501-F83F-8843-BE62-17970C2DA381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AD6D6B-B8A3-4D76-8B04-F2F73E584C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,25 @@
     <sheet name="key_output_weights" sheetId="9" r:id="rId10"/>
     <sheet name="scenario_weights" sheetId="10" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
   <si>
     <t>configuration</t>
   </si>
@@ -38,9 +51,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>use_theme_weights</t>
-  </si>
-  <si>
     <t>key_output</t>
   </si>
   <si>
@@ -179,18 +189,6 @@
     <t>operator</t>
   </si>
   <si>
-    <t>maximum_effect</t>
-  </si>
-  <si>
-    <t>accessibility</t>
-  </si>
-  <si>
-    <t>probability_of_success</t>
-  </si>
-  <si>
-    <t>saturation_point</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -201,9 +199,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>squeezed *</t>
   </si>
   <si>
     <t>Scenarios</t>
@@ -395,13 +390,64 @@
   </si>
   <si>
     <t>Evaluate options by assessing risk appetite</t>
+  </si>
+  <si>
+    <t>AR_1</t>
+  </si>
+  <si>
+    <t>AR_2</t>
+  </si>
+  <si>
+    <t>AR_3</t>
+  </si>
+  <si>
+    <t>AR_4</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>AR_me</t>
+  </si>
+  <si>
+    <t>AR_acc</t>
+  </si>
+  <si>
+    <t>AR_pos</t>
+  </si>
+  <si>
+    <t>AR_sp</t>
+  </si>
+  <si>
+    <t>WURWE_1</t>
+  </si>
+  <si>
+    <t>WURWE_2</t>
+  </si>
+  <si>
+    <t>WURWE_3</t>
+  </si>
+  <si>
+    <t>WURWE_4</t>
+  </si>
+  <si>
+    <t>WURWE_me</t>
+  </si>
+  <si>
+    <t>WURWE_acc</t>
+  </si>
+  <si>
+    <t>WURWE_pos</t>
+  </si>
+  <si>
+    <t>WURWE_sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +485,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -486,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -500,7 +552,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,18 +855,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,20 +874,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -852,35 +895,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -899,35 +942,35 @@
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -946,255 +989,255 @@
       <selection sqref="A1:B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="163.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="B25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1207,34 +1250,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4671918-A843-C04F-9129-57BE941EA328}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.83203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="238" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="220.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
     </row>
   </sheetData>
@@ -1250,43 +1293,43 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1301,12 +1344,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1321,12 +1364,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1354,80 +1397,80 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
       <c r="C2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>250000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
       </c>
       <c r="C5">
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>150000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>150000</v>
@@ -1442,84 +1485,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="C2">
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4">
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>0.9</v>
@@ -1532,60 +1578,124 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>7500000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>15000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14">
+        <v>275000</v>
       </c>
     </row>
   </sheetData>
@@ -1595,222 +1705,301 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2">
-        <v>0.48</v>
-      </c>
-      <c r="F2">
-        <v>0.95</v>
-      </c>
-      <c r="G2">
-        <v>0.9</v>
-      </c>
-      <c r="H2">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3">
-        <v>0.5</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>275000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1823,35 +2012,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>3</v>

</xml_diff>

<commit_message>
clean-up dev for release
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aweijden002\Documents\tRBS anne\Fork Ruen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AD6D6B-B8A3-4D76-8B04-F2F73E584C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A29D46D-61FF-5144-9E3D-34F7F8E5FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="1200" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>configuration</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>threshold</t>
   </si>
   <si>
     <t>Accidents reduction</t>
@@ -857,16 +854,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,12 +871,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -895,35 +892,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -942,35 +939,35 @@
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -986,258 +983,258 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="163.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="B17" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1254,30 +1251,30 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
   </sheetData>
@@ -1287,15 +1284,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1320,16 +1317,13 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1344,12 +1338,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1364,12 +1358,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1397,80 +1391,80 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>250000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>150000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>150000</v>
@@ -1489,83 +1483,83 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2">
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0.9</v>
@@ -1584,115 +1578,115 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>7500000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>15000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>300000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14">
         <v>275000</v>
@@ -1711,291 +1705,291 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>115</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>124</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>126</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>125</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2012,35 +2006,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>

</xml_diff>

<commit_message>
clean-up dev for release (#89)
* clean-up dev for release

* set demo case to beerwiser

---------

Co-authored-by: Thom-Ivar van Dijk <thomivar@gmail.com>
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aweijden002\Documents\tRBS anne\Fork Ruen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7AD6D6B-B8A3-4D76-8B04-F2F73E584C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A29D46D-61FF-5144-9E3D-34F7F8E5FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="1200" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>configuration</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>threshold</t>
   </si>
   <si>
     <t>Accidents reduction</t>
@@ -857,16 +854,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -874,12 +871,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -895,35 +892,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -942,35 +939,35 @@
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -986,258 +983,258 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B31"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="163.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="163.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="B17" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="3" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1254,30 +1251,30 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="220.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
   </sheetData>
@@ -1287,15 +1284,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1320,16 +1317,13 @@
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1344,12 +1338,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1364,12 +1358,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1397,80 +1391,80 @@
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>250000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>250000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
       </c>
       <c r="C5">
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>150000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>150000</v>
@@ -1489,83 +1483,83 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2">
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3">
         <v>0.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>0.9</v>
@@ -1584,115 +1578,115 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>7500000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>15000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>0.95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10">
         <v>300000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14">
         <v>275000</v>
@@ -1711,291 +1705,291 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>115</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>116</v>
-      </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>124</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>126</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>125</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2012,35 +2006,35 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>3</v>

</xml_diff>

<commit_message>
add dict from excel and only optimize when name
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Documents/Aangepast_report/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A29D46D-61FF-5144-9E3D-34F7F8E5FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE03BC-1ABF-F349-B656-B2DB645A1DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1200" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36860" yWindow="1060" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="143">
   <si>
     <t>configuration</t>
   </si>
@@ -438,6 +438,42 @@
   </si>
   <si>
     <t>WURWE_sp</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>report_title_page</t>
+  </si>
+  <si>
+    <t>report_strategic_challenge</t>
+  </si>
+  <si>
+    <t>report_key_outputs_theme</t>
+  </si>
+  <si>
+    <t>report_decision_makers_options</t>
+  </si>
+  <si>
+    <t>report_scenarios</t>
+  </si>
+  <si>
+    <t>report_fixed_inputs</t>
+  </si>
+  <si>
+    <t>report_dependencies</t>
+  </si>
+  <si>
+    <t>report_weighted_appreciations</t>
+  </si>
+  <si>
+    <t>report_add_optimize</t>
+  </si>
+  <si>
+    <t>Optimize_DMO_name</t>
+  </si>
+  <si>
+    <t>DMO_optimized_test</t>
   </si>
 </sst>
 </file>
@@ -551,8 +587,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1FD10895-72A3-7148-9AC0-E24F8F49DC8D}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -852,15 +888,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -877,6 +914,86 @@
       </c>
       <c r="B2" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified the excells with configs and add NEMO
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Documents/Aangepast_report/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EE03BC-1ABF-F349-B656-B2DB645A1DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE6D3D3-124D-7E4A-9694-B6D36F4ECACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36860" yWindow="1060" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="34560" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="144">
   <si>
     <t>configuration</t>
   </si>
@@ -473,7 +473,10 @@
     <t>Optimize_DMO_name</t>
   </si>
   <si>
-    <t>DMO_optimized_test</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Optimized_DMO</t>
   </si>
 </sst>
 </file>
@@ -890,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -921,7 +924,7 @@
         <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -977,7 +980,7 @@
         <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -993,7 +996,7 @@
         <v>140</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flexible tables in PDF and configurations to include/exclude parts in the report (#117)
* make reports flex, add step 7, update colors

* add possibility to include optimize in report

* add dict from excel and only optimize when name

* Error in isnan fixed

* modified the excells with configs and add NEMO

* Same fix DSM but also for JSON en CSV

* add hardcoded page_dict functionality

---------

Co-authored-by: mike.verdaasdonk <mike.verdaasdonk@admin.pwc.com>
</commit_message>
<xml_diff>
--- a/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
+++ b/src/vlinder/data/Beerwiser/xlsx/Beerwiser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tdijk004/Documents/Tooling/vlinder/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mverdaasdo001/Documents/Aangepast_report/trbs/src/vlinder/data/Beerwiser/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A29D46D-61FF-5144-9E3D-34F7F8E5FF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE6D3D3-124D-7E4A-9694-B6D36F4ECACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1200" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="300" windowWidth="34560" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="144">
   <si>
     <t>configuration</t>
   </si>
@@ -438,6 +438,45 @@
   </si>
   <si>
     <t>WURWE_sp</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>report_title_page</t>
+  </si>
+  <si>
+    <t>report_strategic_challenge</t>
+  </si>
+  <si>
+    <t>report_key_outputs_theme</t>
+  </si>
+  <si>
+    <t>report_decision_makers_options</t>
+  </si>
+  <si>
+    <t>report_scenarios</t>
+  </si>
+  <si>
+    <t>report_fixed_inputs</t>
+  </si>
+  <si>
+    <t>report_dependencies</t>
+  </si>
+  <si>
+    <t>report_weighted_appreciations</t>
+  </si>
+  <si>
+    <t>report_add_optimize</t>
+  </si>
+  <si>
+    <t>Optimize_DMO_name</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Optimized_DMO</t>
   </si>
 </sst>
 </file>
@@ -551,8 +590,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1FD10895-72A3-7148-9AC0-E24F8F49DC8D}"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -852,15 +891,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -877,6 +917,86 @@
       </c>
       <c r="B2" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1286,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>